<commit_message>
更新至V2.2.0 refactor: 优化BigDecimalConverter和CellReader实现 feat: 新增LongConverter类 perf: 提升Excel导出和导入的性能体验 refactor: 移除并整合CellReaderResult和TitleReaderResult，添加数据读取和错误处理逻辑 feat: 新增大数据量导入场景优化方法 feat(excel-import): 添加debugger模式并优化sheet索引处理
</commit_message>
<xml_diff>
--- a/excel-utils-example/src/main/resources/导入测试.xlsx
+++ b/excel-utils-example/src/main/resources/导入测试.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12420"/>
+    <workbookView windowHeight="17655" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <r>
       <rPr>
@@ -122,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -155,42 +168,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -231,6 +208,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -276,7 +268,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,49 +310,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,121 +448,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,21 +501,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -535,6 +533,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -593,148 +606,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -745,64 +758,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1104,8 +1117,8 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="D1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -1143,13 +1156,13 @@
       <c r="C2" s="1">
         <v>74</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>45074.7336574074</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>45074.7336574074</v>
       </c>
     </row>
@@ -1163,13 +1176,13 @@
       <c r="C3" s="1">
         <v>75</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>45074.7336574074</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>45074.7336574074</v>
       </c>
     </row>
@@ -1183,13 +1196,13 @@
       <c r="C4" s="1">
         <v>76</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>45074.7336574074</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>45074.7336574074</v>
       </c>
     </row>
@@ -1206,10 +1219,10 @@
       <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>45074.7336574074</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>45074.7336574074</v>
       </c>
     </row>
@@ -1229,14 +1242,65 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="17.125"/>
+    <col min="2" max="2" width="37.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2">
+        <v>45074.7336574074</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2">
+        <v>45074.7336574074</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2">
+        <v>45074.7336574074</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2">
+        <v>45074.7336574074</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="zhangsan@qq.com"/>
+    <hyperlink ref="B3" r:id="rId2" display="lisi@qq.com"/>
+    <hyperlink ref="B4" r:id="rId3" display="wangwu@qq.com"/>
+    <hyperlink ref="B5" r:id="rId4" display="zhaoliu@qq.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
fix(ExampleController): 修正导入逻辑和异常处理 feat(ExTriConsumer): 新增ExTriConsumer接口 refactor(HutoolTitleReader): 重构读取逻辑并新增方法 refactor(TitleReader): 重构read方法并新增抽象方法
</commit_message>
<xml_diff>
--- a/excel-utils-example/src/main/resources/导入测试.xlsx
+++ b/excel-utils-example/src/main/resources/导入测试.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12420"/>
+    <workbookView windowHeight="17655" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <r>
       <rPr>
@@ -122,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -155,42 +168,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -231,6 +208,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -276,7 +268,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,49 +310,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,121 +448,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -488,21 +501,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -535,6 +533,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -593,148 +606,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -745,64 +758,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="10" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1104,8 +1117,8 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="D1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -1143,13 +1156,13 @@
       <c r="C2" s="1">
         <v>74</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>45074.7336574074</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>45074.7336574074</v>
       </c>
     </row>
@@ -1163,13 +1176,13 @@
       <c r="C3" s="1">
         <v>75</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>45074.7336574074</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>45074.7336574074</v>
       </c>
     </row>
@@ -1183,13 +1196,13 @@
       <c r="C4" s="1">
         <v>76</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>45074.7336574074</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>45074.7336574074</v>
       </c>
     </row>
@@ -1206,10 +1219,10 @@
       <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>45074.7336574074</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>45074.7336574074</v>
       </c>
     </row>
@@ -1229,14 +1242,65 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="17.125"/>
+    <col min="2" max="2" width="37.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2">
+        <v>45074.7336574074</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2">
+        <v>45074.7336574074</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2">
+        <v>45074.7336574074</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2">
+        <v>45074.7336574074</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="zhangsan@qq.com"/>
+    <hyperlink ref="B3" r:id="rId2" display="lisi@qq.com"/>
+    <hyperlink ref="B4" r:id="rId3" display="wangwu@qq.com"/>
+    <hyperlink ref="B5" r:id="rId4" display="zhaoliu@qq.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>